<commit_message>
Importing translations using automation
</commit_message>
<xml_diff>
--- a/src/assets/i18n/i18n.xlsx
+++ b/src/assets/i18n/i18n.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Drive\Trabajo\3.ingenieria_informatica\Personal\4.cuarto\tfg\Intentos\corpuser\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08970F24-D3EA-4A45-A5B7-CBB9FB7C2EFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE960B30-1E5E-49B7-92EB-D2B84B52583F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E313C4BE-127E-4B18-A835-432101F769E6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E313C4BE-127E-4B18-A835-432101F769E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>key</t>
   </si>
@@ -57,10 +57,115 @@
     <t>app.navBar.visualizeData</t>
   </si>
   <si>
-    <t>Hola</t>
-  </si>
-  <si>
-    <t>Hello</t>
+    <t>menu.intro.title</t>
+  </si>
+  <si>
+    <t>menu.intro.first_paragraph</t>
+  </si>
+  <si>
+    <t>menu.intro.second_paragraph</t>
+  </si>
+  <si>
+    <t>menu.indexList.title</t>
+  </si>
+  <si>
+    <t>menu.indexList.subtitle</t>
+  </si>
+  <si>
+    <t>menu.indexList.create</t>
+  </si>
+  <si>
+    <t>menu.indexList.documents</t>
+  </si>
+  <si>
+    <t>menu.indexList.creating</t>
+  </si>
+  <si>
+    <t>Gestión de Corpus Documentales</t>
+  </si>
+  <si>
+    <t>Idioma</t>
+  </si>
+  <si>
+    <t>Inicio</t>
+  </si>
+  <si>
+    <t>Añadir documentos</t>
+  </si>
+  <si>
+    <t>Visualizar datos</t>
+  </si>
+  <si>
+    <t>Bienvenido al servicio web de visualización gráfica de conjuntos de datos</t>
+  </si>
+  <si>
+    <t>El mundo de la información evoluciona. Nos vemos obligados cada día a adaptar nuestra tecnología a la oleada de cantidades de datos cada vez más extensas. A la vez que aumenta la necesidad de generar sistemas que aseguren su protección y capacidad de salvaguarda, es necesario el desarrollo de nuevos servicios que nos permitan conocer de una manera auxiliar y sencilla las características de los conjuntos de información que poseemos.</t>
+  </si>
+  <si>
+    <t>Por ello, este proyecto, desarrollado inicialmente como un Trabajo de Fin de Grado, pretende poner de manifiesto las utilidades llevadas por tecnologías web que nos permiten analizar nuestros propios corpus documentales, por medio de gráficas interactivas.</t>
+  </si>
+  <si>
+    <t>Consulta la lista actual de conjuntos en línea</t>
+  </si>
+  <si>
+    <t>Selecciona un corpus para empezar</t>
+  </si>
+  <si>
+    <t>… o crea un nuevo índice</t>
+  </si>
+  <si>
+    <t>Crear</t>
+  </si>
+  <si>
+    <t>documentos</t>
+  </si>
+  <si>
+    <t>Creando el índice…</t>
+  </si>
+  <si>
+    <t>Documental Corpus Management</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Add documents</t>
+  </si>
+  <si>
+    <t>Visualize data</t>
+  </si>
+  <si>
+    <t>Welcome to your dataset graphic visualization web service.</t>
+  </si>
+  <si>
+    <t>The world of global information is evolving. Everyday, we're forced to adapt our technological environment for upcoming waves of extensive data amounts. At the same time it's necessary to generate system to protect information, it's necessary to develop new services to access our documents' most important characteristics, in the simplest of ways.</t>
+  </si>
+  <si>
+    <t>Because of that, this project - developed initially as a final university degree project - tries to manifest the ultimate web techonologies features which permit us to analyze our own documental corpuses using interactive graphs.</t>
+  </si>
+  <si>
+    <t>Check the current online index list</t>
+  </si>
+  <si>
+    <t>Select a corpus to begin</t>
+  </si>
+  <si>
+    <t>… or create a new one</t>
+  </si>
+  <si>
+    <t>documents</t>
+  </si>
+  <si>
+    <t>Creating index…</t>
+  </si>
+  <si>
+    <t>menu.indexList.inputPlaceholder</t>
   </si>
 </sst>
 </file>
@@ -412,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CF3A58-B0D4-4393-BEB3-313DC305A00D}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -441,10 +546,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -452,10 +557,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -463,10 +568,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -474,10 +579,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -485,10 +590,109 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding translations for Upload and Stats components
</commit_message>
<xml_diff>
--- a/src/assets/i18n/i18n.xlsx
+++ b/src/assets/i18n/i18n.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Drive\Trabajo\3.ingenieria_informatica\Personal\4.cuarto\tfg\Intentos\corpuser\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE960B30-1E5E-49B7-92EB-D2B84B52583F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E27B88-8459-421F-9579-E45C14A58589}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E313C4BE-127E-4B18-A835-432101F769E6}"/>
+    <workbookView xWindow="50310" yWindow="3210" windowWidth="14400" windowHeight="7365" xr2:uid="{E313C4BE-127E-4B18-A835-432101F769E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,16 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
-  <si>
-    <t>key</t>
-  </si>
-  <si>
-    <t>es</t>
-  </si>
-  <si>
-    <t>en</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>app.name</t>
   </si>
@@ -166,6 +157,195 @@
   </si>
   <si>
     <t>menu.indexList.inputPlaceholder</t>
+  </si>
+  <si>
+    <t>upload.title</t>
+  </si>
+  <si>
+    <t>Gestiona los documentos que componen tu corpus desde esta página</t>
+  </si>
+  <si>
+    <t>Manage the documents from your dataset in this page</t>
+  </si>
+  <si>
+    <t>upload.elasticConnection</t>
+  </si>
+  <si>
+    <t>Conexión al servidor de Elasticsearch</t>
+  </si>
+  <si>
+    <t>Elasticsearch server connection</t>
+  </si>
+  <si>
+    <t>upload.uploader.addInfo</t>
+  </si>
+  <si>
+    <t>Añade información</t>
+  </si>
+  <si>
+    <t>Add information</t>
+  </si>
+  <si>
+    <t>upload.uploader.uploadDocuments</t>
+  </si>
+  <si>
+    <t>Sube documentos al corpus</t>
+  </si>
+  <si>
+    <t>Upload documents to corpus</t>
+  </si>
+  <si>
+    <t>upload.uploader.drag</t>
+  </si>
+  <si>
+    <t>Arrastra los documentos aquí</t>
+  </si>
+  <si>
+    <t>Drag your documents here</t>
+  </si>
+  <si>
+    <t>upload.uploader.choose</t>
+  </si>
+  <si>
+    <t>Elige los ficheros</t>
+  </si>
+  <si>
+    <t>Choose files</t>
+  </si>
+  <si>
+    <t>upload.uploader.queue</t>
+  </si>
+  <si>
+    <t>Cola de almacenamiento</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>upload.uploader.stillNoFiles</t>
+  </si>
+  <si>
+    <t>Todavía nmo se han añadido documentos.</t>
+  </si>
+  <si>
+    <t>Still no added files.</t>
+  </si>
+  <si>
+    <t>common.name</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>common.format</t>
+  </si>
+  <si>
+    <t>Formato</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>common.options</t>
+  </si>
+  <si>
+    <t>Opciones</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>upload.uploader.remove</t>
+  </si>
+  <si>
+    <t>Quitar de la cola</t>
+  </si>
+  <si>
+    <t>Remove from queue</t>
+  </si>
+  <si>
+    <t>upload.uploader.add</t>
+  </si>
+  <si>
+    <t>Añadir al corpus</t>
+  </si>
+  <si>
+    <t>Add to corpus</t>
+  </si>
+  <si>
+    <t>upload.uploader.addAll</t>
+  </si>
+  <si>
+    <t>Añadir todo</t>
+  </si>
+  <si>
+    <t>Add all</t>
+  </si>
+  <si>
+    <t>upload.uploader.emptyCorpus</t>
+  </si>
+  <si>
+    <t>El corpus está vacío.</t>
+  </si>
+  <si>
+    <t>Corpus is empty</t>
+  </si>
+  <si>
+    <t>upload.uploader.cleanCorpus</t>
+  </si>
+  <si>
+    <t>Borrar datos del corpus</t>
+  </si>
+  <si>
+    <t>Clean corpus</t>
+  </si>
+  <si>
+    <t>stats.title</t>
+  </si>
+  <si>
+    <t>Consulta la información sobre el índice</t>
+  </si>
+  <si>
+    <t>Check information about index</t>
+  </si>
+  <si>
+    <t>stats.filterBar.filters</t>
+  </si>
+  <si>
+    <t>Filtros</t>
+  </si>
+  <si>
+    <t>Filters</t>
+  </si>
+  <si>
+    <t>stats.filterBar.noFiltersAvailable</t>
+  </si>
+  <si>
+    <t>Por el momento no hay filtros aplicables.</t>
+  </si>
+  <si>
+    <t>No active filters for the moment.</t>
+  </si>
+  <si>
+    <t>stats.searchBar.search</t>
+  </si>
+  <si>
+    <t>Busca términos dentro del corpus</t>
+  </si>
+  <si>
+    <t>Search terms inside the corpus</t>
+  </si>
+  <si>
+    <t>KEY</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>EN</t>
   </si>
 </sst>
 </file>
@@ -517,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CF3A58-B0D4-4393-BEB3-313DC305A00D}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -532,167 +712,387 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
         <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Applying translations for project views
</commit_message>
<xml_diff>
--- a/src/assets/i18n/i18n.xlsx
+++ b/src/assets/i18n/i18n.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Drive\Trabajo\3.ingenieria_informatica\Personal\4.cuarto\tfg\Intentos\corpuser\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E27B88-8459-421F-9579-E45C14A58589}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6DE90D-57F1-43FA-A671-D171CE94DA94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50310" yWindow="3210" windowWidth="14400" windowHeight="7365" xr2:uid="{E313C4BE-127E-4B18-A835-432101F769E6}"/>
+    <workbookView xWindow="43200" yWindow="3210" windowWidth="14400" windowHeight="7365" xr2:uid="{E313C4BE-127E-4B18-A835-432101F769E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t>app.name</t>
   </si>
@@ -225,9 +225,6 @@
     <t>upload.uploader.stillNoFiles</t>
   </si>
   <si>
-    <t>Todavía nmo se han añadido documentos.</t>
-  </si>
-  <si>
     <t>Still no added files.</t>
   </si>
   <si>
@@ -346,6 +343,45 @@
   </si>
   <si>
     <t>EN</t>
+  </si>
+  <si>
+    <t>Todavía no se han añadido documentos.</t>
+  </si>
+  <si>
+    <t>Actualizando las visualizaciones. Un momento…</t>
+  </si>
+  <si>
+    <t>Loading visualizations. Please wait…</t>
+  </si>
+  <si>
+    <t>fragments.loadingSpinner.loading</t>
+  </si>
+  <si>
+    <t>fragments.titleList.title</t>
+  </si>
+  <si>
+    <t>Lista de documentos</t>
+  </si>
+  <si>
+    <t>Document list</t>
+  </si>
+  <si>
+    <t>fragments.titleList.find</t>
+  </si>
+  <si>
+    <t>Encuentra documentos</t>
+  </si>
+  <si>
+    <t>Find documents</t>
+  </si>
+  <si>
+    <t>fragments.titleList.noDocuments</t>
+  </si>
+  <si>
+    <t>No hay documentos disponibles.</t>
+  </si>
+  <si>
+    <t>There are no available documents.</t>
   </si>
 </sst>
 </file>
@@ -697,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CF3A58-B0D4-4393-BEB3-313DC305A00D}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -712,13 +748,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
         <v>102</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>103</v>
-      </c>
-      <c r="C1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -957,142 +993,186 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" t="s">
         <v>64</v>
-      </c>
-      <c r="C23" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
         <v>66</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>67</v>
-      </c>
-      <c r="C24" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
         <v>69</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>70</v>
-      </c>
-      <c r="C25" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" t="s">
         <v>72</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>73</v>
-      </c>
-      <c r="C26" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
         <v>75</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>76</v>
-      </c>
-      <c r="C27" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" t="s">
         <v>78</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>79</v>
-      </c>
-      <c r="C28" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" t="s">
         <v>81</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>82</v>
-      </c>
-      <c r="C29" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" t="s">
         <v>84</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>85</v>
-      </c>
-      <c r="C30" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" t="s">
         <v>87</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>88</v>
-      </c>
-      <c r="C31" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" t="s">
         <v>90</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>91</v>
-      </c>
-      <c r="C32" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" t="s">
         <v>93</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>94</v>
-      </c>
-      <c r="C33" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" t="s">
         <v>96</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>97</v>
-      </c>
-      <c r="C34" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" t="s">
         <v>99</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>100</v>
       </c>
-      <c r="C35" t="s">
-        <v>101</v>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pending literals to translate
</commit_message>
<xml_diff>
--- a/src/assets/i18n/i18n.xlsx
+++ b/src/assets/i18n/i18n.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Drive\Trabajo\3.ingenieria_informatica\Personal\4.cuarto\tfg\Intentos\corpuser\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6DE90D-57F1-43FA-A671-D171CE94DA94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45A1330-480A-4FE2-AD56-36504B422C84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43200" yWindow="3210" windowWidth="14400" windowHeight="7365" xr2:uid="{E313C4BE-127E-4B18-A835-432101F769E6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t>app.name</t>
   </si>
@@ -382,6 +382,42 @@
   </si>
   <si>
     <t>There are no available documents.</t>
+  </si>
+  <si>
+    <t>fragments.topicsGraph.title</t>
+  </si>
+  <si>
+    <t>Ideas principales</t>
+  </si>
+  <si>
+    <t>Main topics</t>
+  </si>
+  <si>
+    <t>fragments.docsPerYearGraph.docCount</t>
+  </si>
+  <si>
+    <t>fragments.docsPerYearGraph.title</t>
+  </si>
+  <si>
+    <t>Cronología del corpus</t>
+  </si>
+  <si>
+    <t>Corpus time line</t>
+  </si>
+  <si>
+    <t>Número de documentos</t>
+  </si>
+  <si>
+    <t>Document count</t>
+  </si>
+  <si>
+    <t>fragments.docsPerYearGraph.postDate</t>
+  </si>
+  <si>
+    <t>Año de publicación</t>
+  </si>
+  <si>
+    <t>Year of publication</t>
   </si>
 </sst>
 </file>
@@ -733,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CF3A58-B0D4-4393-BEB3-313DC305A00D}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1175,7 +1211,52 @@
         <v>116</v>
       </c>
     </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>